<commit_message>
added code for certificate generation with duratio
</commit_message>
<xml_diff>
--- a/certificate_pdf/data/student_details.xlsx
+++ b/certificate_pdf/data/student_details.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -33,25 +33,22 @@
     <t xml:space="preserve">Date</t>
   </si>
   <si>
-    <t xml:space="preserve">Aakash Tiwari</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Python</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patel pashwa milindkumar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">React JS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DHRUMIK MUKESHBHAI PATEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GHANCHI MUHAMMEDFAIZAL USMANBHAI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Harshil Dave</t>
+    <t xml:space="preserve">Duration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vishvajeet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DataScience with Python and PowerBi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 Days Internship</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vishvajeet.vnurture@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -62,7 +59,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -94,6 +91,13 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="0"/>
@@ -107,18 +111,12 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -155,7 +153,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -164,23 +162,27 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -261,17 +263,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -284,61 +288,45 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" s="4" t="n">
         <v>44720</v>
       </c>
+      <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="4" t="n">
-        <v>44721</v>
-      </c>
-    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="4" t="n">
-        <v>44722</v>
-      </c>
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="4" t="n">
-        <v>44723</v>
-      </c>
+      <c r="A5" s="7"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="4" t="n">
-        <v>44724</v>
-      </c>
+      <c r="A6" s="7"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -396,6 +384,9 @@
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" display="vishvajeet.vnurture@gmail.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -417,7 +408,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -440,7 +431,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>